<commit_message>
define DataTable req MBI1
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F29D798C-6DA9-481D-934B-08833900550C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772D5C59-1540-4244-B42B-39FBAFAE51C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTableBDD" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Step</t>
   </si>
@@ -46,15 +46,6 @@
     <t>Scenario1</t>
   </si>
   <si>
-    <t>V2.1</t>
-  </si>
-  <si>
-    <t>ParamName4</t>
-  </si>
-  <si>
-    <t>2021/4/30</t>
-  </si>
-  <si>
     <t>set excel file</t>
   </si>
   <si>
@@ -89,13 +80,151 @@
   </si>
   <si>
     <t>Check count</t>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Header2</t>
+  </si>
+  <si>
+    <t>Header3</t>
+  </si>
+  <si>
+    <t>Header4</t>
+  </si>
+  <si>
+    <t>Header5</t>
+  </si>
+  <si>
+    <t>Header6</t>
+  </si>
+  <si>
+    <t>Header7</t>
+  </si>
+  <si>
+    <t>Header8</t>
+  </si>
+  <si>
+    <t>Value1.1</t>
+  </si>
+  <si>
+    <t>Value2.1</t>
+  </si>
+  <si>
+    <t>Value3.1</t>
+  </si>
+  <si>
+    <t>Value1.2</t>
+  </si>
+  <si>
+    <t>Value1.3</t>
+  </si>
+  <si>
+    <t>Value1.4</t>
+  </si>
+  <si>
+    <t>Value1.5</t>
+  </si>
+  <si>
+    <t>Value1.6</t>
+  </si>
+  <si>
+    <t>Value1.7</t>
+  </si>
+  <si>
+    <t>Value1.8</t>
+  </si>
+  <si>
+    <t>Value2.2</t>
+  </si>
+  <si>
+    <t>Value2.3</t>
+  </si>
+  <si>
+    <t>Value2.4</t>
+  </si>
+  <si>
+    <t>Value2.5</t>
+  </si>
+  <si>
+    <t>Value2.6</t>
+  </si>
+  <si>
+    <t>Value2.7</t>
+  </si>
+  <si>
+    <t>Value2.8</t>
+  </si>
+  <si>
+    <t>Value3.2</t>
+  </si>
+  <si>
+    <t>Value3.3</t>
+  </si>
+  <si>
+    <t>Value3.4</t>
+  </si>
+  <si>
+    <t>Value3.5</t>
+  </si>
+  <si>
+    <t>Value3.6</t>
+  </si>
+  <si>
+    <t>Value3.7</t>
+  </si>
+  <si>
+    <t>Value3.8</t>
+  </si>
+  <si>
+    <t>DataTable1</t>
+  </si>
+  <si>
+    <t>DataTableBDD.xlsx</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>MandatoryColumn</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>V0.3</t>
+  </si>
+  <si>
+    <t>V0.4</t>
+  </si>
+  <si>
+    <t>Set input</t>
+  </si>
+  <si>
+    <t>FirstGridValue</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>LastGridValue</t>
+  </si>
+  <si>
+    <t>V4.4</t>
+  </si>
+  <si>
+    <t>Check Other Parameters</t>
+  </si>
+  <si>
+    <t>ColumnCount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +241,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,8 +274,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -162,11 +304,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -176,8 +386,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,120 +729,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
-  <dimension ref="A4:D13"/>
+  <dimension ref="A4:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="6" t="s">
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="11"/>
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="6" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="13"/>
+      <c r="B11" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="3">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -614,12 +904,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE645D2-4AB9-494E-A144-2E25D55D5616}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
try to deploy java, and add ps datatable
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E105856\ExcelBDD\ExcelBDD\BDDExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F517DE-55FA-4B21-859D-FD73C8F790B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F4352A-DC8C-4F49-BBB1-55E05F66A19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTableBDD" sheetId="1" r:id="rId1"/>
     <sheet name="DataTable1" sheetId="2" r:id="rId2"/>
+    <sheet name="DataTable2" sheetId="3" r:id="rId3"/>
+    <sheet name="DataTable3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="91">
   <si>
     <t>Step</t>
   </si>
@@ -186,15 +189,9 @@
     <t>FirstGridValue</t>
   </si>
   <si>
-    <t>V1.1</t>
-  </si>
-  <si>
     <t>LastGridValue</t>
   </si>
   <si>
-    <t>V4.4</t>
-  </si>
-  <si>
     <t>Check Other Parameters</t>
   </si>
   <si>
@@ -289,6 +286,30 @@
   </si>
   <si>
     <t>Value8.6</t>
+  </si>
+  <si>
+    <t>set Start column</t>
+  </si>
+  <si>
+    <t>StartColumn</t>
+  </si>
+  <si>
+    <t>Scenario2</t>
+  </si>
+  <si>
+    <t>DataTable2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Scenario3</t>
+  </si>
+  <si>
+    <t>DataTable3</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -451,8 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -486,9 +505,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,7 +529,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -800,22 +825,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
-  <dimension ref="A4:E13"/>
+  <dimension ref="A4:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,143 +856,220 @@
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="9" t="s">
+      <c r="F4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="10"/>
-      <c r="B6" s="6" t="s">
+      <c r="F5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="8"/>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="10"/>
-      <c r="B7" s="6" t="s">
+      <c r="F6" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="8"/>
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="16">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="10"/>
-      <c r="B8" s="6" t="s">
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="8"/>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="11"/>
-      <c r="B9" s="6" t="s">
+      <c r="F8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8"/>
+      <c r="B9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="9"/>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="12" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="F11" s="16">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="11"/>
+      <c r="B12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="6" t="s">
+      <c r="E13" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="12"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="E14" s="16">
+        <v>8</v>
+      </c>
+      <c r="F14" s="16">
+        <v>8</v>
+      </c>
+      <c r="G14" s="16">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -982,188 +1084,188 @@
       <selection activeCell="D3" sqref="D3:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:8">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1171,4 +1273,412 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C32F4F0-7755-446C-AE9F-5F1F1CFB967B}">
+  <dimension ref="B1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141B375C-AE87-4361-B116-C9E6E6630FDC}">
+  <dimension ref="C3:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="3:10">
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10">
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AF3944-1ABD-4A54-9484-D9BD8FD651BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
switch to old Get-ExcelWorksheet for datatable
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7785E6CD-335A-41E2-BDFD-A8ECB930E5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC9CB43-BEB0-437B-9569-F536B5CDE455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTableBDD" sheetId="1" r:id="rId1"/>
     <sheet name="DataTable1" sheetId="2" r:id="rId2"/>
     <sheet name="DataTable2" sheetId="3" r:id="rId3"/>
     <sheet name="DataTable3" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
+    <sheet name="DataTableV0.5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="90">
   <si>
     <t>Step</t>
   </si>
@@ -298,6 +299,15 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>V0.5</t>
+  </si>
+  <si>
+    <t>Check same header, same header should be collected by another name, for example, the 2nd Header's key is Header2, the 3rd Header's key is Header3, if end with number, then increase the number</t>
+  </si>
+  <si>
+    <t>DataTableV0.5</t>
   </si>
 </sst>
 </file>
@@ -445,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -484,6 +494,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
-  <dimension ref="A4:G12"/>
+  <dimension ref="A4:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,9 +828,10 @@
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,8 +853,11 @@
       <c r="G4" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="9" t="s">
         <v>44</v>
       </c>
@@ -859,8 +879,11 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -880,8 +903,11 @@
       <c r="G6" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="10"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -901,8 +927,11 @@
       <c r="G7" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="10"/>
       <c r="B8" s="4" t="s">
         <v>79</v>
@@ -922,8 +951,11 @@
       <c r="G8" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -945,8 +977,11 @@
       <c r="G9" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="14" t="s">
         <v>47</v>
@@ -966,8 +1001,11 @@
       <c r="G10" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="4" t="s">
@@ -985,8 +1023,11 @@
       <c r="G11" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
       <c r="C12" s="4" t="s">
@@ -1003,6 +1044,17 @@
       </c>
       <c r="G12" s="7">
         <v>8</v>
+      </c>
+      <c r="H12" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="120">
+      <c r="B13" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1011,6 +1063,7 @@
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B10:B12"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1021,7 +1074,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1612,6 +1665,203 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192235F0-7F41-4E8C-B5F6-D90DB65886FD}">
+  <dimension ref="A2:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AF3944-1ABD-4A54-9484-D9BD8FD651BC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
support duplicated headers in PowerShell
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC9CB43-BEB0-437B-9569-F536B5CDE455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669D0826-41FC-4C29-86B3-FD4CAA8981C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="92">
   <si>
     <t>Step</t>
   </si>
@@ -79,30 +79,6 @@
     <t>Check count</t>
   </si>
   <si>
-    <t>Header1</t>
-  </si>
-  <si>
-    <t>Header2</t>
-  </si>
-  <si>
-    <t>Header3</t>
-  </si>
-  <si>
-    <t>Header4</t>
-  </si>
-  <si>
-    <t>Header5</t>
-  </si>
-  <si>
-    <t>Header6</t>
-  </si>
-  <si>
-    <t>Header7</t>
-  </si>
-  <si>
-    <t>Header8</t>
-  </si>
-  <si>
     <t>Value1.1</t>
   </si>
   <si>
@@ -304,10 +280,40 @@
     <t>V0.5</t>
   </si>
   <si>
-    <t>Check same header, same header should be collected by another name, for example, the 2nd Header's key is Header2, the 3rd Header's key is Header3, if end with number, then increase the number</t>
-  </si>
-  <si>
     <t>DataTableV0.5</t>
+  </si>
+  <si>
+    <t>Header01</t>
+  </si>
+  <si>
+    <t>Header02</t>
+  </si>
+  <si>
+    <t>Header03</t>
+  </si>
+  <si>
+    <t>Header04</t>
+  </si>
+  <si>
+    <t>Header05</t>
+  </si>
+  <si>
+    <t>Header06</t>
+  </si>
+  <si>
+    <t>Header07</t>
+  </si>
+  <si>
+    <t>Header08</t>
+  </si>
+  <si>
+    <t>Read depulicated header</t>
+  </si>
+  <si>
+    <t>Header03InThirdSet</t>
+  </si>
+  <si>
+    <t>Check same header, same header should be collected by another name, for example, the 2nd Header's key is Header02, the 3rd Header's key is Header03, if end with number, then increase the number</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -500,6 +506,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +830,7 @@
   <dimension ref="A4:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -839,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -848,39 +860,39 @@
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -889,22 +901,22 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -913,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
@@ -934,25 +946,25 @@
     <row r="8" spans="1:8">
       <c r="A8" s="10"/>
       <c r="B8" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -963,7 +975,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
@@ -984,57 +996,57 @@
     <row r="10" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E12" s="7">
         <v>8</v>
@@ -1050,11 +1062,29 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="120">
+      <c r="A13" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="B13" s="17" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1074,191 +1104,191 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1273,191 +1303,191 @@
   <dimension ref="B1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" s="6" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:9">
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1471,191 +1501,191 @@
   <dimension ref="C3:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:10">
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="3:10">
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="3:10">
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="3:10">
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="3:10">
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="3:10">
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="3:10">
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1669,191 +1699,191 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to use MS Excel
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669D0826-41FC-4C29-86B3-FD4CAA8981C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A9A9F0-D545-4F7B-BE4D-ED2764F666C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTableBDD" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="95">
   <si>
     <t>Step</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>Check same header, same header should be collected by another name, for example, the 2nd Header's key is Header02, the 3rd Header's key is Header03, if end with number, then increase the number</t>
+  </si>
+  <si>
+    <t>notes:</t>
+  </si>
+  <si>
+    <t>this is not collected by ExcellBDD</t>
+  </si>
+  <si>
+    <t>notes: this is not collected by ExcellBDD</t>
   </si>
 </sst>
 </file>
@@ -477,6 +486,18 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,18 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,7 +839,7 @@
   <dimension ref="A4:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -870,7 +879,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -896,7 +905,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="10"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -915,12 +924,12 @@
       <c r="G6" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="10"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -944,7 +953,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="10"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>71</v>
       </c>
@@ -968,7 +977,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -994,8 +1003,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1018,8 +1027,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
@@ -1040,8 +1049,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1062,16 +1071,16 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="120">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="12" t="s">
         <v>90</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1101,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE645D2-4AB9-494E-A144-2E25D55D5616}">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1289,6 +1298,14 @@
       </c>
       <c r="H8" s="5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1300,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C32F4F0-7755-446C-AE9F-5F1F1CFB967B}">
-  <dimension ref="B1:I7"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1488,6 +1505,11 @@
       </c>
       <c r="I7" s="5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1498,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141B375C-AE87-4361-B116-C9E6E6630FDC}">
-  <dimension ref="C3:J9"/>
+  <dimension ref="C3:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1686,6 +1708,11 @@
       </c>
       <c r="J9" s="5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
+      <c r="C11" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1696,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192235F0-7F41-4E8C-B5F6-D90DB65886FD}">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1884,6 +1911,11 @@
       </c>
       <c r="H8" s="5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to release V0.5 on PS
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A9A9F0-D545-4F7B-BE4D-ED2764F666C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80098BD4-050F-4E14-9112-5B391925AFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>set Header row</t>
   </si>
   <si>
-    <t>get test set list</t>
-  </si>
-  <si>
     <t>TestSetCount</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>Header03InThirdSet</t>
   </si>
   <si>
-    <t>Check same header, same header should be collected by another name, for example, the 2nd Header's key is Header02, the 3rd Header's key is Header03, if end with number, then increase the number</t>
-  </si>
-  <si>
     <t>notes:</t>
   </si>
   <si>
@@ -323,6 +317,12 @@
   </si>
   <si>
     <t>notes: this is not collected by ExcellBDD</t>
+  </si>
+  <si>
+    <t>get testset list</t>
+  </si>
+  <si>
+    <t>any duplicated header should be collected by another name, for example, the 2nd Header's key is Header02, the 3rd Header's key is Header03, if the duplicated ends with 2 number,such as 03, then increase the number.</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,8 +385,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -409,68 +421,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -486,41 +441,36 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,14 +788,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
   <dimension ref="A4:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="19.42578125" customWidth="1"/>
@@ -857,10 +807,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -869,75 +819,75 @@
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="13" t="s">
-        <v>36</v>
+      <c r="A5" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
@@ -953,41 +903,41 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="E9" s="7">
         <v>6</v>
@@ -1003,59 +953,59 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="16"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="18"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="18"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="16"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="7">
         <v>8</v>
@@ -1071,29 +1021,29 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="120">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>27</v>
+      <c r="E13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1112,200 +1062,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE645D2-4AB9-494E-A144-2E25D55D5616}">
   <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1327,189 +1277,189 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:9">
       <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1530,189 +1480,189 @@
   <sheetData>
     <row r="3" spans="3:10">
       <c r="C3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="3:10">
       <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="3:10">
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="3:10">
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="3:10">
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="3:10">
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="3:10">
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="3:10">
       <c r="C11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1725,197 +1675,197 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192235F0-7F41-4E8C-B5F6-D90DB65886FD}">
   <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pass 1st test on openxml
</commit_message>
<xml_diff>
--- a/BDDExcel/DataTableBDD.xlsx
+++ b/BDDExcel/DataTableBDD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7803EC-E978-4E09-A255-F44F6C01B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B249E32C-C62C-4EA1-8C06-30C209D7143E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{513EC524-C410-4B00-B12F-D02046789CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTableBDD" sheetId="1" r:id="rId1"/>
@@ -789,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6FFDF-A533-45DE-AE30-7B256E237E30}">
-  <dimension ref="A4:H16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -805,6 +805,21 @@
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>0</v>
@@ -1068,14 +1083,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE645D2-4AB9-494E-A144-2E25D55D5616}">
-  <dimension ref="A2:H10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>80</v>

</xml_diff>